<commit_message>
Update PDF and Xlsx
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valentinslr-my.sharepoint.com/personal/hello_valentinslr_com/Documents/Documents/GitHub/script-nsg/httpget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{D894E5D9-125F-427A-8D95-FE59EEB2AFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{551459F2-B13C-44F7-968F-BD4F9D857651}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C690B0CE-0A75-4F2F-A76A-9D3169BED32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="297">
   <si>
     <t>Country</t>
   </si>
@@ -909,6 +909,24 @@
   </si>
   <si>
     <t>SRR (SFR Réunion)_10Gbps_FR.xml</t>
+  </si>
+  <si>
+    <t>Vultr (1Gbps, London, UK).xml</t>
+  </si>
+  <si>
+    <t>Vultr (London)</t>
+  </si>
+  <si>
+    <t>Vultr (Manchester)</t>
+  </si>
+  <si>
+    <t>Vultr (1Gbps, Manchester, UK).xml</t>
+  </si>
+  <si>
+    <t>Vultr Paris</t>
+  </si>
+  <si>
+    <t>Vultr (1Gbps, Paris, FR).xml</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1251,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>0.84552845528455289</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>0.15447154471544716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2362,10 +2380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,7 +2413,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.8666666666666667</v>
+        <v>0.84552845528455289</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2419,7 +2437,7 @@
       </c>
       <c r="H2" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.13333333333333333</v>
+        <v>0.15447154471544716</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3752,19 +3770,19 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>18</v>
+        <v>295</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>19</v>
+        <v>296</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3772,13 +3790,13 @@
         <v>17</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>14</v>
@@ -3789,13 +3807,13 @@
         <v>17</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>230</v>
+        <v>26</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>14</v>
@@ -3806,13 +3824,13 @@
         <v>17</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>14</v>
@@ -3823,13 +3841,13 @@
         <v>17</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>14</v>
@@ -3840,13 +3858,13 @@
         <v>17</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>167</v>
+        <v>232</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>14</v>
@@ -3854,16 +3872,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>14</v>
@@ -3871,50 +3889,50 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>61</v>
+        <v>292</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>63</v>
+        <v>291</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>227</v>
+        <v>17</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>228</v>
+        <v>293</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>229</v>
+        <v>68</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>227</v>
+        <v>162</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>249</v>
+        <v>163</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>250</v>
+      <c r="D90" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>14</v>
@@ -3922,16 +3940,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>239</v>
+        <v>60</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>240</v>
+        <v>61</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>241</v>
+        <v>62</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>14</v>
@@ -3939,16 +3957,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>208</v>
+        <v>62</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>14</v>
@@ -3956,16 +3974,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>136</v>
+        <v>227</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>137</v>
+        <v>249</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>138</v>
+      <c r="D93" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>14</v>
@@ -3973,16 +3991,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>136</v>
+        <v>239</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>140</v>
+        <v>68</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>14</v>
@@ -3990,16 +4008,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>14</v>
@@ -4007,50 +4025,50 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>278</v>
+        <v>136</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>279</v>
+        <v>137</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>280</v>
+        <v>138</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>263</v>
+        <v>136</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>262</v>
+        <v>139</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>281</v>
+        <v>140</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>14</v>
@@ -4058,50 +4076,50 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>9</v>
+        <v>279</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>8</v>
+        <v>280</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>10</v>
+        <v>263</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>101</v>
+        <v>262</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>102</v>
+        <v>281</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>14</v>
@@ -4112,13 +4130,13 @@
         <v>10</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>182</v>
+        <v>9</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>183</v>
+        <v>8</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>14</v>
@@ -4126,16 +4144,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>14</v>
@@ -4143,16 +4161,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>14</v>
@@ -4160,16 +4178,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>14</v>
@@ -4180,13 +4198,13 @@
         <v>22</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>14</v>
@@ -4194,16 +4212,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>14</v>
@@ -4211,16 +4229,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>166</v>
+        <v>209</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>14</v>
@@ -4228,16 +4246,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>14</v>
@@ -4245,16 +4263,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>14</v>
@@ -4262,16 +4280,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>14</v>
@@ -4279,16 +4297,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>29</v>
+        <v>213</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>30</v>
+        <v>214</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>14</v>
@@ -4296,16 +4314,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>14</v>
@@ -4313,16 +4331,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>14</v>
@@ -4333,13 +4351,13 @@
         <v>28</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>236</v>
+        <v>29</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>237</v>
+        <v>27</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>238</v>
+        <v>30</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>14</v>
@@ -4350,13 +4368,13 @@
         <v>28</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>14</v>
@@ -4367,13 +4385,13 @@
         <v>28</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>14</v>
@@ -4381,16 +4399,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>27</v>
+        <v>237</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>14</v>
@@ -4398,16 +4416,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>14</v>
@@ -4415,16 +4433,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>14</v>
@@ -4435,15 +4453,66 @@
         <v>57</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>94</v>
+        <v>225</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D121" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D124" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E124" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add some PT Server
</commit_message>
<xml_diff>
--- a/httpget/List File.xlsx
+++ b/httpget/List File.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\script-nsg\httpget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valentinslr-my.sharepoint.com/personal/hello_valentinslr_com/Documents/Documents/GitHub/script-nsg/httpget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32EA29B-9A5A-42B0-91A7-2476963FDAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F32EA29B-9A5A-42B0-91A7-2476963FDAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50E96E3A-96E9-49D7-A62B-1633CB64BFB7}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{DC6502BA-425D-411E-B718-7BD70301C676}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="364">
   <si>
     <t>Country</t>
   </si>
@@ -1107,6 +1107,27 @@
   </si>
   <si>
     <t>G-Core ZA_10Gbps_ZA.xml</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>NOS Lisboa</t>
+  </si>
+  <si>
+    <t>NOS_10Gbps_Lisboa_PT.xml</t>
+  </si>
+  <si>
+    <t>NOS Porto</t>
+  </si>
+  <si>
+    <t>NOS_10Gbps_Porto_PT.xml</t>
+  </si>
+  <si>
+    <t>DataPacket</t>
+  </si>
+  <si>
+    <t>DataPacket_10Gbps_Lisboa_PT.xml</t>
   </si>
 </sst>
 </file>
@@ -1358,6 +1379,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0394-47C0-AC6D-34B828EA7B25}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1450,10 +1476,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.72972972972972971</c:v>
+                  <c:v>0.71523178807947019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27027027027027029</c:v>
+                  <c:v>0.28476821192052981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2579,10 +2605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C18607A-68F6-4C8B-BF40-82CCB3747CF3}">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,7 +2638,7 @@
       </c>
       <c r="H1" s="1">
         <f>COUNTIF(E:E,"Yes")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.72972972972972971</v>
+        <v>0.71523178807947019</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2654,7 +2680,7 @@
       </c>
       <c r="H3" s="1">
         <f>COUNTIF(E:E,"No")/SUM(COUNTIF(E:E,"Yes"),COUNTIF(E:E,"No"))</f>
-        <v>0.27027027027027029</v>
+        <v>0.28476821192052981</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4684,53 +4710,53 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>22</v>
+        <v>357</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>35</v>
+        <v>362</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>36</v>
+        <v>363</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>22</v>
+        <v>357</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>23</v>
+        <v>358</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>25</v>
+        <v>359</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>22</v>
+        <v>357</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>210</v>
+        <v>360</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>209</v>
+        <v>361</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4738,13 +4764,13 @@
         <v>22</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>14</v>
@@ -4752,33 +4778,33 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>336</v>
+        <v>23</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>337</v>
+        <v>25</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>14</v>
@@ -4786,16 +4812,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>14</v>
@@ -4806,30 +4832,30 @@
         <v>87</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>213</v>
+        <v>336</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>214</v>
+        <v>337</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>14</v>
@@ -4837,33 +4863,33 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>338</v>
+        <v>87</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>339</v>
+        <v>165</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>340</v>
+        <v>166</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>145</v>
+        <v>213</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>14</v>
@@ -4871,67 +4897,67 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>341</v>
+        <v>141</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>342</v>
+        <v>142</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>343</v>
+        <v>143</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>28</v>
+        <v>338</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>29</v>
+        <v>339</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>30</v>
+        <v>340</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>346</v>
+        <v>145</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>350</v>
+        <v>146</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>28</v>
+        <v>341</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>15</v>
@@ -4942,16 +4968,16 @@
         <v>28</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>348</v>
+        <v>29</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>352</v>
+        <v>30</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4959,13 +4985,13 @@
         <v>28</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>15</v>
@@ -4976,16 +5002,16 @@
         <v>28</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>78</v>
+        <v>347</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>79</v>
+        <v>351</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4993,16 +5019,16 @@
         <v>28</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>85</v>
+        <v>348</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>86</v>
+        <v>352</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -5010,16 +5036,16 @@
         <v>28</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>236</v>
+        <v>349</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>237</v>
+        <v>6</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>238</v>
+        <v>353</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -5027,13 +5053,13 @@
         <v>28</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>14</v>
@@ -5044,13 +5070,13 @@
         <v>28</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>171</v>
+        <v>85</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>14</v>
@@ -5058,33 +5084,33 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>354</v>
+        <v>28</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>6</v>
+        <v>237</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>356</v>
+        <v>238</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>14</v>
@@ -5092,16 +5118,16 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>14</v>
@@ -5109,19 +5135,19 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>57</v>
+        <v>354</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>72</v>
+        <v>355</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>73</v>
+        <v>356</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5129,15 +5155,66 @@
         <v>57</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>94</v>
+        <v>225</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D149" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D152" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E149" s="2" t="s">
+      <c r="E152" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>